<commit_message>
store patent, news data in DB
</commit_message>
<xml_diff>
--- a/preprocessing/dart/company_info.xlsx
+++ b/preprocessing/dart/company_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanah\Desktop\workspace\Project\ESG\preprocessing\dart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F88BB65-00B7-490B-8901-1F30F0CD825C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F000D1-B148-4696-AB09-B2E1B2D1E16D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16384,17 +16384,7 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -16751,8 +16741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1369" workbookViewId="0">
-      <selection activeCell="L1378" sqref="L1378"/>
+    <sheetView tabSelected="1" topLeftCell="A1215" workbookViewId="0">
+      <selection activeCell="L1228" sqref="L1228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>

</xml_diff>